<commit_message>
[ADD] add permission of syncuserws
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hrds_code_repo/hzero_platform/hzero-menu-user-role-label.xlsx
+++ b/src/main/resources/script/db/init-data/hrds_code_repo/hzero_platform/hzero-menu-user-role-label.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="597" activeTab="6"/>
+    <workbookView windowWidth="19485" windowHeight="8460" tabRatio="597" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="435">
   <si>
     <r>
       <rPr>
@@ -2431,6 +2431,15 @@
   </si>
   <si>
     <t>code-repo-service.rdm-member-applicant-proj.batchRefuse</t>
+  </si>
+  <si>
+    <t>iam_menu_permission-57</t>
+  </si>
+  <si>
+    <t>code-repo-service.rdm-member.syncBatchMember</t>
+  </si>
+  <si>
+    <t>iam_menu_permission-58</t>
   </si>
   <si>
     <t>标签表</t>
@@ -3155,14 +3164,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3177,17 +3201,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3201,7 +3239,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3215,10 +3268,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3231,13 +3301,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -3245,61 +3308,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3399,7 +3408,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3417,13 +3462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3435,7 +3474,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3447,7 +3534,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3459,115 +3570,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3680,36 +3689,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3730,25 +3719,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3773,155 +3753,184 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4404,21 +4413,21 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15.5833333333333" style="17" customWidth="1"/>
+    <col min="1" max="1" width="15.5851851851852" style="17" customWidth="1"/>
     <col min="2" max="2" width="10.3333333333333" style="18" customWidth="1"/>
-    <col min="3" max="3" width="28.1666666666667" customWidth="1"/>
+    <col min="3" max="3" width="28.162962962963" customWidth="1"/>
     <col min="4" max="4" width="35.3333333333333" style="13" customWidth="1"/>
-    <col min="5" max="5" width="38.5833333333333" customWidth="1"/>
-    <col min="6" max="6" width="23.4166666666667" customWidth="1"/>
-    <col min="7" max="7" width="21.5833333333333" customWidth="1"/>
+    <col min="5" max="5" width="38.5851851851852" customWidth="1"/>
+    <col min="6" max="6" width="23.4148148148148" customWidth="1"/>
+    <col min="7" max="7" width="21.5851851851852" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.5833333333333" customWidth="1"/>
+    <col min="9" max="9" width="24.5851851851852" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="19.1666666666667" customWidth="1"/>
-    <col min="12" max="12" width="18.5833333333333" customWidth="1"/>
-    <col min="13" max="13" width="13.1666666666667" customWidth="1"/>
+    <col min="11" max="11" width="19.162962962963" customWidth="1"/>
+    <col min="12" max="12" width="18.5851851851852" customWidth="1"/>
+    <col min="13" max="13" width="13.1703703703704" customWidth="1"/>
     <col min="14" max="1025" width="10.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4433,7 +4442,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="5:5">
+    <row r="2" ht="18" spans="5:5">
       <c r="E2" s="22"/>
     </row>
     <row r="3" ht="49.5" customHeight="1" spans="3:7">
@@ -4447,7 +4456,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" ht="18" spans="3:7">
       <c r="C4" s="25" t="s">
         <v>3</v>
       </c>
@@ -4468,7 +4477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" ht="18" spans="3:5">
       <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
@@ -4488,7 +4497,7 @@
       </c>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" ht="52.2" spans="3:6">
+    <row r="9" ht="51.75" spans="3:6">
       <c r="C9" s="35" t="s">
         <v>13</v>
       </c>
@@ -4502,7 +4511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="52.2" spans="3:5">
+    <row r="10" ht="51.75" spans="3:5">
       <c r="C10" s="38" t="s">
         <v>17</v>
       </c>
@@ -4513,7 +4522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="69.6" spans="3:5">
+    <row r="11" ht="69" spans="3:5">
       <c r="C11" s="32" t="s">
         <v>20</v>
       </c>
@@ -4545,7 +4554,7 @@
       <c r="D14" s="33"/>
       <c r="E14" s="34"/>
     </row>
-    <row r="15" ht="34.8" spans="3:5">
+    <row r="15" ht="34.5" spans="3:5">
       <c r="C15" s="40" t="s">
         <v>26</v>
       </c>
@@ -4568,7 +4577,7 @@
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" ht="18" spans="3:4">
       <c r="C20" s="44" t="s">
         <v>31</v>
       </c>
@@ -4576,7 +4585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" ht="18" spans="3:4">
       <c r="C21" s="44" t="s">
         <v>33</v>
       </c>
@@ -4584,7 +4593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" ht="18" spans="3:4">
       <c r="C22" s="44" t="s">
         <v>35</v>
       </c>
@@ -4592,7 +4601,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" ht="18" spans="3:4">
       <c r="C23" s="44" t="s">
         <v>37</v>
       </c>
@@ -4618,7 +4627,7 @@
       </c>
       <c r="E26" s="23"/>
     </row>
-    <row r="27" ht="52.2" spans="3:3">
+    <row r="27" ht="51.75" spans="3:3">
       <c r="C27" s="46" t="s">
         <v>43</v>
       </c>
@@ -4645,17 +4654,18 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
     <col min="5" max="5" width="16.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="54.75" customWidth="1"/>
-    <col min="7" max="7" width="15.25" customWidth="1"/>
-    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="6" max="6" width="66.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="21.7777777777778" customWidth="1"/>
+    <col min="10" max="10" width="23.1111111111111" customWidth="1"/>
+    <col min="11" max="11" width="16.7481481481481" customWidth="1"/>
     <col min="15" max="15" width="29.6666666666667" customWidth="1"/>
-    <col min="16" max="16" width="45.8333333333333" customWidth="1"/>
+    <col min="16" max="16" width="45.8296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5375,17 +5385,17 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="6"/>
   <cols>
-    <col min="5" max="5" width="21.25" customWidth="1"/>
-    <col min="6" max="6" width="17.5833333333333" customWidth="1"/>
-    <col min="7" max="7" width="58.75" customWidth="1"/>
+    <col min="5" max="5" width="24.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="17.5851851851852" customWidth="1"/>
+    <col min="7" max="7" width="58.7481481481481" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6022,6 +6032,30 @@
       </c>
       <c r="G56" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7">
+      <c r="E57" t="s">
+        <v>231</v>
+      </c>
+      <c r="F57" t="str">
+        <f>菜单SAAS版!E18</f>
+        <v>iam_menu-19</v>
+      </c>
+      <c r="G57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7">
+      <c r="E58" t="s">
+        <v>233</v>
+      </c>
+      <c r="F58" t="str">
+        <f>菜单SAAS版!$E$11</f>
+        <v>iam_menu-11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -6036,18 +6070,18 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="5" max="5" width="26.5833333333333" customWidth="1"/>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="17.4166666666667" customWidth="1"/>
-    <col min="8" max="8" width="21.9166666666667" customWidth="1"/>
-    <col min="11" max="11" width="19.0833333333333" customWidth="1"/>
-    <col min="13" max="13" width="12.75" customWidth="1"/>
-    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="26.5851851851852" customWidth="1"/>
+    <col min="6" max="6" width="25.5037037037037" customWidth="1"/>
+    <col min="7" max="7" width="17.4148148148148" customWidth="1"/>
+    <col min="8" max="8" width="21.9185185185185" customWidth="1"/>
+    <col min="11" max="11" width="19.0814814814815" customWidth="1"/>
+    <col min="13" max="13" width="12.7481481481481" customWidth="1"/>
+    <col min="14" max="14" width="15.5037037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6083,66 +6117,66 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I7" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="L7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="M7" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="N7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="O7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="5:15">
       <c r="E8" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G8" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J8" t="s">
+        <v>250</v>
+      </c>
+      <c r="K8" t="s">
         <v>247</v>
-      </c>
-      <c r="K8" t="s">
-        <v>244</v>
       </c>
       <c r="M8" t="s">
         <v>82</v>
@@ -6156,19 +6190,19 @@
     </row>
     <row r="9" spans="5:15">
       <c r="E9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G9" t="s">
         <v>248</v>
-      </c>
-      <c r="F9" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" t="s">
-        <v>245</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
@@ -6182,25 +6216,25 @@
     </row>
     <row r="10" spans="5:15">
       <c r="E10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F10" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G10" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H10" t="s">
         <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K10" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="M10" t="s">
         <v>82</v>
@@ -6214,19 +6248,19 @@
     </row>
     <row r="11" spans="5:15">
       <c r="E11" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F11" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G11" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H11" t="s">
         <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="M11" t="s">
         <v>82</v>
@@ -6240,25 +6274,25 @@
     </row>
     <row r="12" spans="5:15">
       <c r="E12" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G12" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J12" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="K12" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -6278,33 +6312,33 @@
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="5:9">
       <c r="E15" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F15" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G15" t="str">
         <f>菜单SAAS版!$E$12</f>
@@ -6315,15 +6349,15 @@
         <v>iam_label-11</v>
       </c>
       <c r="I15" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="5:9">
       <c r="E16" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G16" t="str">
         <f>菜单SAAS版!$E$9</f>
@@ -6334,15 +6368,15 @@
         <v>iam_label-8</v>
       </c>
       <c r="I16" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="5:9">
       <c r="E17" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F17" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G17" t="str">
         <f>菜单SAAS版!$E$10</f>
@@ -6353,15 +6387,15 @@
         <v>iam_label-8</v>
       </c>
       <c r="I17" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="5:9">
       <c r="E18" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F18" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G18" t="str">
         <f>菜单SAAS版!$E$11</f>
@@ -6372,15 +6406,15 @@
         <v>iam_label-8</v>
       </c>
       <c r="I18" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="5:9">
       <c r="E19" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G19" t="str">
         <f>菜单SAAS版!$E$13</f>
@@ -6391,15 +6425,15 @@
         <v>iam_label-11</v>
       </c>
       <c r="I19" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="5:9">
       <c r="E20" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F20" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G20" t="str">
         <f>菜单SAAS版!E19</f>
@@ -6410,15 +6444,15 @@
         <v>iam_label-21</v>
       </c>
       <c r="I20" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="5:9">
       <c r="E21" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F21" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G21" t="str">
         <f>菜单SAAS版!E15</f>
@@ -6429,15 +6463,15 @@
         <v>iam_label-21</v>
       </c>
       <c r="I21" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="5:9">
       <c r="E22" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F22" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G22" t="str">
         <f>菜单SAAS版!E8</f>
@@ -6448,7 +6482,7 @@
         <v>iam_label-8</v>
       </c>
       <c r="I22" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -6466,10 +6500,10 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="5" max="5" width="17.8333333333333" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="17.837037037037" customWidth="1"/>
+    <col min="6" max="6" width="22.5037037037037" customWidth="1"/>
     <col min="7" max="7" width="39.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6506,10 +6540,10 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>54</v>
@@ -6524,75 +6558,75 @@
         <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="J7" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="O7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="P7" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="Q7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="R7" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="S7" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="T7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="U7" t="s">
         <v>68</v>
       </c>
       <c r="V7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="X7" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="Y7" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="5:23">
       <c r="E8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F8" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G8" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="I8" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="J8" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="K8" t="s">
         <v>80</v>
@@ -6625,10 +6659,10 @@
         <v>80</v>
       </c>
       <c r="U8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="V8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="W8" t="s">
         <v>80</v>
@@ -6636,19 +6670,19 @@
     </row>
     <row r="9" spans="5:23">
       <c r="E9" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F9" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="G9" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H9" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="I9" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="J9" t="s">
         <v>79</v>
@@ -6684,10 +6718,10 @@
         <v>80</v>
       </c>
       <c r="U9" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="V9" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="W9" t="s">
         <v>80</v>
@@ -6695,16 +6729,16 @@
     </row>
     <row r="10" spans="5:25">
       <c r="E10" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F10" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G10" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H10" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="J10" t="s">
         <v>79</v>
@@ -6741,10 +6775,10 @@
         <v>80</v>
       </c>
       <c r="U10" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="V10" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="W10" t="s">
         <v>80</v>
@@ -6753,21 +6787,21 @@
         <v>100</v>
       </c>
       <c r="Y10" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="5:25">
       <c r="E11" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F11" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G11" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H11" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="J11" t="s">
         <v>79</v>
@@ -6804,33 +6838,33 @@
         <v>80</v>
       </c>
       <c r="U11" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="V11" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="W11" t="s">
         <v>80</v>
       </c>
       <c r="X11" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="Y11" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="5:25">
       <c r="E12" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="G12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H12" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="J12" t="s">
         <v>79</v>
@@ -6867,10 +6901,10 @@
         <v>80</v>
       </c>
       <c r="U12" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="V12" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="W12" t="s">
         <v>80</v>
@@ -6879,21 +6913,21 @@
         <v>129</v>
       </c>
       <c r="Y12" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="5:25">
       <c r="E13" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F13" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G13" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="H13" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="J13" t="s">
         <v>79</v>
@@ -6930,10 +6964,10 @@
         <v>80</v>
       </c>
       <c r="U13" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="V13" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="W13" t="s">
         <v>80</v>
@@ -6942,24 +6976,24 @@
         <v>125</v>
       </c>
       <c r="Y13" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="5:23">
       <c r="E14" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F14" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G14" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="H14" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="J14" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="K14" t="s">
         <v>80</v>
@@ -6993,10 +7027,10 @@
         <v>80</v>
       </c>
       <c r="U14" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="V14" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="W14" t="s">
         <v>80</v>
@@ -7010,33 +7044,33 @@
         <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="H16" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="I16" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="5:10">
       <c r="E17" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F17" t="str">
         <f>角色!$E$10</f>
@@ -7047,18 +7081,18 @@
         <v>iam_menu-10</v>
       </c>
       <c r="H17" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I17" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="5:10">
       <c r="E18" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F18" t="str">
         <f>角色!$E$10</f>
@@ -7069,18 +7103,18 @@
         <v>iam_menu-11</v>
       </c>
       <c r="H18" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I18" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J18" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="5:10">
       <c r="E19" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F19" t="str">
         <f>角色!$E$10</f>
@@ -7091,18 +7125,18 @@
         <v>iam_menu-17</v>
       </c>
       <c r="H19" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I19" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J19" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="5:10">
       <c r="E20" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="F20" t="str">
         <f>角色!$E$10</f>
@@ -7113,18 +7147,18 @@
         <v>iam_menu-18</v>
       </c>
       <c r="H20" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I20" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J20" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="5:10">
       <c r="E21" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F21" t="str">
         <f>角色!$E$10</f>
@@ -7135,18 +7169,18 @@
         <v>iam_menu-19</v>
       </c>
       <c r="H21" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I21" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J21" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="5:10">
       <c r="E22" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F22" t="str">
         <f>角色!$E$10</f>
@@ -7157,18 +7191,18 @@
         <v>iam_menu-14</v>
       </c>
       <c r="H22" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I22" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J22" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="5:10">
       <c r="E23" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F23" t="str">
         <f>角色!$E$11</f>
@@ -7179,18 +7213,18 @@
         <v>iam_menu-14</v>
       </c>
       <c r="H23" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I23" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J23" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="5:10">
       <c r="E24" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F24" t="str">
         <f>角色!$E$12</f>
@@ -7201,18 +7235,18 @@
         <v>iam_menu-17</v>
       </c>
       <c r="H24" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I24" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J24" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="5:10">
       <c r="E25" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F25" t="str">
         <f>角色!$E$12</f>
@@ -7223,18 +7257,18 @@
         <v>iam_menu-19</v>
       </c>
       <c r="H25" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I25" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J25" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="5:10">
       <c r="E26" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="F26" t="str">
         <f>角色!$E$12</f>
@@ -7245,18 +7279,18 @@
         <v>iam_menu-14</v>
       </c>
       <c r="H26" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I26" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J26" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="5:10">
       <c r="E27" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F27" t="str">
         <f>角色!$E$13</f>
@@ -7267,18 +7301,18 @@
         <v>iam_menu-17</v>
       </c>
       <c r="H27" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I27" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J27" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="5:10">
       <c r="E28" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="F28" t="str">
         <f>角色!$E$13</f>
@@ -7289,18 +7323,18 @@
         <v>iam_menu-18</v>
       </c>
       <c r="H28" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I28" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J28" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="5:10">
       <c r="E29" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F29" t="str">
         <f>角色!$E$13</f>
@@ -7311,18 +7345,18 @@
         <v>iam_menu-19</v>
       </c>
       <c r="H29" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I29" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J29" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="5:10">
       <c r="E30" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F30" t="str">
         <f>角色!$E$13</f>
@@ -7333,13 +7367,13 @@
         <v>iam_menu-14</v>
       </c>
       <c r="H30" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I30" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="J30" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -7357,10 +7391,10 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="28.4166666666667" customWidth="1"/>
+    <col min="5" max="5" width="17.5037037037037" customWidth="1"/>
+    <col min="6" max="6" width="28.4148148148148" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7397,66 +7431,66 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I7" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="K7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="L7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="M7" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="N7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="O7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="5:15">
       <c r="E8" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F8" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="G8" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J8" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="K8" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="M8" t="s">
         <v>80</v>
@@ -7470,25 +7504,25 @@
     </row>
     <row r="9" spans="5:15">
       <c r="E9" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G9" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J9" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="K9" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
@@ -7502,25 +7536,25 @@
     </row>
     <row r="10" spans="5:15">
       <c r="E10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F10" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="G10" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H10" t="s">
         <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J10" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="K10" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="M10" t="s">
         <v>80</v>
@@ -7534,25 +7568,25 @@
     </row>
     <row r="11" spans="5:15">
       <c r="E11" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="F11" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G11" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H11" t="s">
         <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J11" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="K11" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="M11" t="s">
         <v>80</v>
@@ -7566,25 +7600,25 @@
     </row>
     <row r="12" spans="5:15">
       <c r="E12" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F12" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="G12" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H12" t="s">
         <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J12" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="K12" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="M12" t="s">
         <v>80</v>
@@ -7598,25 +7632,25 @@
     </row>
     <row r="13" spans="5:15">
       <c r="E13" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="G13" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H13" t="s">
         <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J13" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="K13" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="M13" t="s">
         <v>80</v>
@@ -7630,25 +7664,25 @@
     </row>
     <row r="14" spans="5:15">
       <c r="E14" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="F14" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="G14" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H14" t="s">
         <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J14" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="K14" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="M14" t="s">
         <v>80</v>
@@ -7662,25 +7696,25 @@
     </row>
     <row r="15" spans="5:15">
       <c r="E15" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="F15" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="G15" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H15" t="s">
         <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J15" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="K15" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="M15" t="s">
         <v>80</v>
@@ -7694,25 +7728,25 @@
     </row>
     <row r="16" spans="5:15">
       <c r="E16" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="F16" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="G16" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H16" t="s">
         <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J16" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="K16" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="M16" t="s">
         <v>80</v>
@@ -7726,25 +7760,25 @@
     </row>
     <row r="17" spans="5:15">
       <c r="E17" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F17" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="G17" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="H17" t="s">
         <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J17" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="K17" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="M17" t="s">
         <v>80</v>
@@ -7768,21 +7802,21 @@
   <sheetPr/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="3" max="3" width="18.0833333333333" customWidth="1"/>
+    <col min="3" max="3" width="18.0814814814815" customWidth="1"/>
     <col min="4" max="4" width="19.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="23.4166666666667" customWidth="1"/>
-    <col min="6" max="6" width="29.9166666666667" customWidth="1"/>
-    <col min="7" max="7" width="20.4166666666667" customWidth="1"/>
+    <col min="5" max="5" width="23.4148148148148" customWidth="1"/>
+    <col min="6" max="6" width="29.9185185185185" customWidth="1"/>
+    <col min="7" max="7" width="20.4148148148148" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="23.75" customWidth="1"/>
+    <col min="9" max="9" width="23.7481481481481" customWidth="1"/>
     <col min="10" max="10" width="41.7777777777778" customWidth="1"/>
-    <col min="11" max="11" width="26.4166666666667" customWidth="1"/>
+    <col min="11" max="11" width="26.4148148148148" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:4">
@@ -7816,38 +7850,38 @@
     <row r="6" customFormat="1"/>
     <row r="7" customFormat="1" spans="1:8">
       <c r="A7" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="1" spans="4:7">
       <c r="D8" s="1"/>
       <c r="E8" s="6" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="4:7">
@@ -7870,31 +7904,31 @@
     </row>
     <row r="13" customFormat="1" spans="1:7">
       <c r="A13" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="4:8">
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F14" s="5" t="str">
         <f>菜单SAAS版!E15</f>
@@ -7930,57 +7964,57 @@
     <row r="18" customFormat="1"/>
     <row r="19" customFormat="1" spans="1:11">
       <c r="A19" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H19" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="I19" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="J19" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" s="8" customFormat="1" spans="5:11">
       <c r="E20" s="11" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="I20" s="8">
         <v>119800</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="K20" s="8" t="str">
         <f>菜单SAAS版!E16</f>
@@ -7989,22 +8023,22 @@
     </row>
     <row r="21" s="8" customFormat="1" spans="5:11">
       <c r="E21" s="11" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I21" s="8">
         <v>119824</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="K21" s="8" t="str">
         <f>菜单SAAS版!E16</f>
@@ -8020,33 +8054,33 @@
     <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:8">
       <c r="A25" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="H25" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="5:8">
       <c r="E26" s="6" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="F26" t="str">
         <f>E8</f>
@@ -8062,7 +8096,7 @@
     </row>
     <row r="27" customFormat="1" spans="5:8">
       <c r="E27" s="6" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="F27" t="str">
         <f>E8</f>
@@ -8091,14 +8125,14 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="17.25"/>
   <cols>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
-    <col min="6" max="6" width="20.1666666666667" customWidth="1"/>
-    <col min="7" max="7" width="15.9166666666667" customWidth="1"/>
-    <col min="8" max="8" width="27.1666666666667" customWidth="1"/>
-    <col min="9" max="9" width="30.5833333333333" customWidth="1"/>
-    <col min="10" max="10" width="43.5833333333333" customWidth="1"/>
+    <col min="5" max="5" width="22.2518518518519" customWidth="1"/>
+    <col min="6" max="6" width="20.162962962963" customWidth="1"/>
+    <col min="7" max="7" width="15.9185185185185" customWidth="1"/>
+    <col min="8" max="8" width="27.162962962963" customWidth="1"/>
+    <col min="9" max="9" width="30.5851851851852" customWidth="1"/>
+    <col min="10" max="10" width="43.5851851851852" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8128,37 +8162,37 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="4:9">
       <c r="D8" s="1"/>
       <c r="E8" s="6" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="F8" t="str">
         <f>菜单SAAS版!E15</f>
@@ -8177,7 +8211,7 @@
     <row r="9" spans="4:9">
       <c r="D9" s="1"/>
       <c r="E9" s="6" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="F9" t="str">
         <f>菜单SAAS版!E9</f>

</xml_diff>

<commit_message>
[FIX] fix the menu iocn
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hrds_code_repo/hzero_platform/hzero-menu-user-role-label.xlsx
+++ b/src/main/resources/script/db/init-data/hrds_code_repo/hzero_platform/hzero-menu-user-role-label.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="8460" tabRatio="597" activeTab="2"/>
+    <workbookView windowWidth="19485" windowHeight="8460" tabRatio="597" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -2070,7 +2070,7 @@
     <t>40</t>
   </si>
   <si>
-    <t>manage_person</t>
+    <t>manage_person-o</t>
   </si>
   <si>
     <t>/rducm/personal-setting</t>
@@ -3077,10 +3077,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="45">
     <font>
@@ -3191,6 +3191,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -3220,13 +3227,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -3234,7 +3234,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3242,14 +3250,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3263,11 +3263,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3279,11 +3279,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3296,16 +3311,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3319,23 +3326,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3435,13 +3435,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3459,7 +3471,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3471,19 +3495,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3495,31 +3531,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3531,37 +3549,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3579,37 +3573,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3716,6 +3716,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3779,6 +3788,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3793,171 +3813,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4680,8 +4680,8 @@
   <sheetPr/>
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -5414,7 +5414,7 @@
   <sheetPr/>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D52" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="D52" workbookViewId="0">
       <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>

</xml_diff>